<commit_message>
Updated Player Shot on Target Data
</commit_message>
<xml_diff>
--- a/data/2019MLS_ShotsOnTgt.xlsx
+++ b/data/2019MLS_ShotsOnTgt.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$177</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="228">
   <si>
     <t>Pos</t>
   </si>
@@ -532,6 +532,180 @@
   </si>
   <si>
     <t>RealSaltLake</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Osorio</t>
+  </si>
+  <si>
+    <t>DeLeon</t>
+  </si>
+  <si>
+    <t>HamiltonJor</t>
+  </si>
+  <si>
+    <t>Akinola</t>
+  </si>
+  <si>
+    <t>Altidore</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>DelgadoMar</t>
+  </si>
+  <si>
+    <t>Pozuelo</t>
+  </si>
+  <si>
+    <t>ChapmanJay</t>
+  </si>
+  <si>
+    <t>Laryea</t>
+  </si>
+  <si>
+    <t>MoorDre</t>
+  </si>
+  <si>
+    <t>MorrowJus</t>
+  </si>
+  <si>
+    <t>Ciman</t>
+  </si>
+  <si>
+    <t>Mavinga</t>
+  </si>
+  <si>
+    <t>Katai</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Mihailovic</t>
+  </si>
+  <si>
+    <t>Frankowski</t>
+  </si>
+  <si>
+    <t>Sapong</t>
+  </si>
+  <si>
+    <t>MartinezCri</t>
+  </si>
+  <si>
+    <t>McCarty</t>
+  </si>
+  <si>
+    <t>Hasler</t>
+  </si>
+  <si>
+    <t>Marcelo</t>
+  </si>
+  <si>
+    <t>Nikolic</t>
+  </si>
+  <si>
+    <t>EdwardsRah</t>
+  </si>
+  <si>
+    <t>Herbers</t>
+  </si>
+  <si>
+    <t>Schweinsteiger</t>
+  </si>
+  <si>
+    <t>Gaitan</t>
+  </si>
+  <si>
+    <t>Campos</t>
+  </si>
+  <si>
+    <t>Bronico</t>
+  </si>
+  <si>
+    <t>SmithKyl</t>
+  </si>
+  <si>
+    <t>Kljestan</t>
+  </si>
+  <si>
+    <t>Akindele</t>
+  </si>
+  <si>
+    <t>MuellerChr</t>
+  </si>
+  <si>
+    <t>DwyerDom</t>
+  </si>
+  <si>
+    <t>Ruan</t>
+  </si>
+  <si>
+    <t>Nani</t>
+  </si>
+  <si>
+    <t>Moutinho</t>
+  </si>
+  <si>
+    <t>JohnsonWil</t>
+  </si>
+  <si>
+    <t>Colman</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Auro</t>
+  </si>
+  <si>
+    <t>BoydTer</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Zavaleta</t>
+  </si>
+  <si>
+    <t>Afful</t>
+  </si>
+  <si>
+    <t>Zardes</t>
+  </si>
+  <si>
+    <t>Sauro</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+  </si>
+  <si>
+    <t>Meram</t>
+  </si>
+  <si>
+    <t>Robinho</t>
+  </si>
+  <si>
+    <t>SantosPed</t>
+  </si>
+  <si>
+    <t>Higuain</t>
+  </si>
+  <si>
+    <t>Mensah</t>
+  </si>
+  <si>
+    <t>JimenezHec</t>
+  </si>
+  <si>
+    <t>GuzmanDav</t>
+  </si>
+  <si>
+    <t>WilliamsJJ</t>
   </si>
 </sst>
 </file>
@@ -589,8 +763,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -600,9 +776,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -932,17 +1110,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O142"/>
+  <dimension ref="A1:O198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A141" sqref="A141"/>
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H185" sqref="H185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -7619,8 +7797,2640 @@
         <v>169</v>
       </c>
     </row>
+    <row r="143" spans="1:15">
+      <c r="A143" t="s">
+        <v>21</v>
+      </c>
+      <c r="B143" t="s">
+        <v>170</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="G143">
+        <v>1</v>
+      </c>
+      <c r="H143" s="1">
+        <v>0</v>
+      </c>
+      <c r="I143" s="3">
+        <v>0</v>
+      </c>
+      <c r="J143" s="3">
+        <v>0</v>
+      </c>
+      <c r="K143" s="3">
+        <v>0</v>
+      </c>
+      <c r="L143" s="3">
+        <v>1</v>
+      </c>
+      <c r="M143" s="3">
+        <v>1</v>
+      </c>
+      <c r="N143" s="3">
+        <v>0</v>
+      </c>
+      <c r="O143" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15">
+      <c r="A144" t="s">
+        <v>21</v>
+      </c>
+      <c r="B144" t="s">
+        <v>171</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>2</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>3</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+      <c r="H144" s="1">
+        <v>2</v>
+      </c>
+      <c r="I144" s="3">
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>1</v>
+      </c>
+      <c r="K144" s="3">
+        <v>0</v>
+      </c>
+      <c r="L144" s="3">
+        <v>0</v>
+      </c>
+      <c r="M144" s="3">
+        <v>1</v>
+      </c>
+      <c r="N144">
+        <v>1</v>
+      </c>
+      <c r="O144" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
+      <c r="A145" t="s">
+        <v>21</v>
+      </c>
+      <c r="B145" t="s">
+        <v>172</v>
+      </c>
+      <c r="C145">
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>4</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+      <c r="H145" s="1">
+        <v>2</v>
+      </c>
+      <c r="I145" s="3">
+        <v>0</v>
+      </c>
+      <c r="J145" s="3">
+        <v>0</v>
+      </c>
+      <c r="K145" s="3">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145" s="3">
+        <v>0</v>
+      </c>
+      <c r="N145">
+        <v>2</v>
+      </c>
+      <c r="O145" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15">
+      <c r="A146" t="s">
+        <v>20</v>
+      </c>
+      <c r="B146" t="s">
+        <v>173</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>2</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>5</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+      <c r="H146" s="1">
+        <v>3</v>
+      </c>
+      <c r="I146" s="3">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146">
+        <v>0</v>
+      </c>
+      <c r="M146" s="3">
+        <v>0</v>
+      </c>
+      <c r="N146">
+        <v>2</v>
+      </c>
+      <c r="O146" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15">
+      <c r="A147" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>1</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147" s="1">
+        <v>2</v>
+      </c>
+      <c r="I147" s="3">
+        <v>0</v>
+      </c>
+      <c r="J147" s="3">
+        <v>0</v>
+      </c>
+      <c r="K147" s="3">
+        <v>0</v>
+      </c>
+      <c r="L147" s="3">
+        <v>0</v>
+      </c>
+      <c r="M147" s="3">
+        <v>0</v>
+      </c>
+      <c r="N147">
+        <v>1</v>
+      </c>
+      <c r="O147" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15">
+      <c r="A148" t="s">
+        <v>20</v>
+      </c>
+      <c r="B148" t="s">
+        <v>175</v>
+      </c>
+      <c r="C148">
+        <v>2</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>1</v>
+      </c>
+      <c r="G148">
+        <v>2</v>
+      </c>
+      <c r="H148" s="1">
+        <v>3</v>
+      </c>
+      <c r="I148" s="3">
+        <v>1</v>
+      </c>
+      <c r="J148" s="3">
+        <v>0</v>
+      </c>
+      <c r="K148" s="3">
+        <v>0</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148" s="3">
+        <v>0</v>
+      </c>
+      <c r="N148">
+        <v>3</v>
+      </c>
+      <c r="O148" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15">
+      <c r="A149" t="s">
+        <v>21</v>
+      </c>
+      <c r="B149" t="s">
+        <v>177</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+      <c r="H149" s="1">
+        <v>1</v>
+      </c>
+      <c r="I149" s="3">
+        <v>0</v>
+      </c>
+      <c r="J149" s="3">
+        <v>0</v>
+      </c>
+      <c r="K149" s="3">
+        <v>0</v>
+      </c>
+      <c r="L149" s="3">
+        <v>0</v>
+      </c>
+      <c r="M149" s="3">
+        <v>0</v>
+      </c>
+      <c r="N149" s="3">
+        <v>0</v>
+      </c>
+      <c r="O149" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15">
+      <c r="A150" t="s">
+        <v>21</v>
+      </c>
+      <c r="B150" t="s">
+        <v>178</v>
+      </c>
+      <c r="C150">
+        <v>3</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>3</v>
+      </c>
+      <c r="F150">
+        <v>5</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
+      </c>
+      <c r="H150" s="1">
+        <v>3</v>
+      </c>
+      <c r="I150">
+        <v>2</v>
+      </c>
+      <c r="J150" s="3">
+        <v>0</v>
+      </c>
+      <c r="K150" s="3">
+        <v>0</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150">
+        <v>1</v>
+      </c>
+      <c r="N150">
+        <v>1</v>
+      </c>
+      <c r="O150" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15">
+      <c r="A151" t="s">
+        <v>21</v>
+      </c>
+      <c r="B151" t="s">
+        <v>179</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151" s="1">
+        <v>1</v>
+      </c>
+      <c r="I151" s="3">
+        <v>0</v>
+      </c>
+      <c r="J151" s="3">
+        <v>0</v>
+      </c>
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151">
+        <v>0</v>
+      </c>
+      <c r="N151">
+        <v>1</v>
+      </c>
+      <c r="O151" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15">
+      <c r="A152" t="s">
+        <v>21</v>
+      </c>
+      <c r="B152" t="s">
+        <v>180</v>
+      </c>
+      <c r="C152">
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152" s="1">
+        <v>0</v>
+      </c>
+      <c r="I152" s="3">
+        <v>0</v>
+      </c>
+      <c r="J152" s="3">
+        <v>0</v>
+      </c>
+      <c r="K152" s="3">
+        <v>0</v>
+      </c>
+      <c r="L152" s="3">
+        <v>0</v>
+      </c>
+      <c r="M152" s="3">
+        <v>0</v>
+      </c>
+      <c r="N152" s="3">
+        <v>0</v>
+      </c>
+      <c r="O152" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15">
+      <c r="A153" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" t="s">
+        <v>181</v>
+      </c>
+      <c r="C153">
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153" s="1">
+        <v>0</v>
+      </c>
+      <c r="I153" s="3">
+        <v>0</v>
+      </c>
+      <c r="J153" s="3">
+        <v>0</v>
+      </c>
+      <c r="K153" s="3">
+        <v>0</v>
+      </c>
+      <c r="L153" s="3">
+        <v>0</v>
+      </c>
+      <c r="M153" s="3">
+        <v>0</v>
+      </c>
+      <c r="N153" s="3">
+        <v>0</v>
+      </c>
+      <c r="O153" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15">
+      <c r="A154" t="s">
+        <v>26</v>
+      </c>
+      <c r="B154" t="s">
+        <v>182</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>2</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154" s="1">
+        <v>0</v>
+      </c>
+      <c r="I154" s="3">
+        <v>0</v>
+      </c>
+      <c r="J154" s="3">
+        <v>0</v>
+      </c>
+      <c r="K154" s="3">
+        <v>0</v>
+      </c>
+      <c r="L154" s="3">
+        <v>0</v>
+      </c>
+      <c r="M154" s="3">
+        <v>0</v>
+      </c>
+      <c r="N154" s="3">
+        <v>0</v>
+      </c>
+      <c r="O154" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15">
+      <c r="A155" t="s">
+        <v>26</v>
+      </c>
+      <c r="B155" t="s">
+        <v>183</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155" s="1">
+        <v>0</v>
+      </c>
+      <c r="I155" s="3">
+        <v>0</v>
+      </c>
+      <c r="J155" s="3">
+        <v>0</v>
+      </c>
+      <c r="K155" s="3">
+        <v>0</v>
+      </c>
+      <c r="L155" s="3">
+        <v>0</v>
+      </c>
+      <c r="M155" s="3">
+        <v>0</v>
+      </c>
+      <c r="N155" s="3">
+        <v>0</v>
+      </c>
+      <c r="O155" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15">
+      <c r="A156" t="s">
+        <v>26</v>
+      </c>
+      <c r="B156" t="s">
+        <v>184</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>2</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156" s="1">
+        <v>0</v>
+      </c>
+      <c r="I156" s="3">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3">
+        <v>0</v>
+      </c>
+      <c r="K156" s="3">
+        <v>0</v>
+      </c>
+      <c r="L156" s="3">
+        <v>0</v>
+      </c>
+      <c r="M156" s="3">
+        <v>0</v>
+      </c>
+      <c r="N156" s="3">
+        <v>0</v>
+      </c>
+      <c r="O156" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15">
+      <c r="A157" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" t="s">
+        <v>212</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>2</v>
+      </c>
+      <c r="H157" s="1">
+        <v>0</v>
+      </c>
+      <c r="I157" s="3">
+        <v>0</v>
+      </c>
+      <c r="J157" s="3">
+        <v>0</v>
+      </c>
+      <c r="K157" s="3">
+        <v>0</v>
+      </c>
+      <c r="L157" s="3">
+        <v>0</v>
+      </c>
+      <c r="M157" s="3">
+        <v>0</v>
+      </c>
+      <c r="N157" s="3">
+        <v>0</v>
+      </c>
+      <c r="O157" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15">
+      <c r="A158" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" t="s">
+        <v>213</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158" s="1">
+        <v>0</v>
+      </c>
+      <c r="I158" s="3">
+        <v>0</v>
+      </c>
+      <c r="J158" s="3">
+        <v>0</v>
+      </c>
+      <c r="K158" s="3">
+        <v>0</v>
+      </c>
+      <c r="L158" s="3">
+        <v>0</v>
+      </c>
+      <c r="M158" s="3">
+        <v>0</v>
+      </c>
+      <c r="N158" s="3">
+        <v>0</v>
+      </c>
+      <c r="O158" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15">
+      <c r="A159" t="s">
+        <v>26</v>
+      </c>
+      <c r="B159" t="s">
+        <v>215</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159" s="1">
+        <v>0</v>
+      </c>
+      <c r="I159" s="3">
+        <v>0</v>
+      </c>
+      <c r="J159" s="3">
+        <v>0</v>
+      </c>
+      <c r="K159" s="3">
+        <v>0</v>
+      </c>
+      <c r="L159" s="3">
+        <v>0</v>
+      </c>
+      <c r="M159" s="3">
+        <v>0</v>
+      </c>
+      <c r="N159" s="3">
+        <v>0</v>
+      </c>
+      <c r="O159" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15">
+      <c r="A160" t="s">
+        <v>21</v>
+      </c>
+      <c r="B160" t="s">
+        <v>214</v>
+      </c>
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160" s="1">
+        <v>0</v>
+      </c>
+      <c r="I160" s="3">
+        <v>0</v>
+      </c>
+      <c r="J160" s="3">
+        <v>0</v>
+      </c>
+      <c r="K160" s="3">
+        <v>0</v>
+      </c>
+      <c r="L160" s="3">
+        <v>0</v>
+      </c>
+      <c r="M160" s="3">
+        <v>0</v>
+      </c>
+      <c r="N160" s="3">
+        <v>0</v>
+      </c>
+      <c r="O160" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15">
+      <c r="A161" t="s">
+        <v>21</v>
+      </c>
+      <c r="B161" t="s">
+        <v>185</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+      <c r="D161">
+        <v>3</v>
+      </c>
+      <c r="E161">
+        <v>5</v>
+      </c>
+      <c r="F161">
+        <v>3</v>
+      </c>
+      <c r="G161">
+        <v>2</v>
+      </c>
+      <c r="H161" s="2">
+        <v>3</v>
+      </c>
+      <c r="I161" s="3">
+        <v>0</v>
+      </c>
+      <c r="J161" s="3">
+        <v>0</v>
+      </c>
+      <c r="K161" s="3">
+        <v>0</v>
+      </c>
+      <c r="L161" s="3">
+        <v>1</v>
+      </c>
+      <c r="M161" s="3">
+        <v>0</v>
+      </c>
+      <c r="N161" s="3">
+        <v>2</v>
+      </c>
+      <c r="O161" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15">
+      <c r="A162" t="s">
+        <v>21</v>
+      </c>
+      <c r="B162" t="s">
+        <v>187</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>2</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+      <c r="H162" s="2">
+        <v>1</v>
+      </c>
+      <c r="I162" s="3">
+        <v>0</v>
+      </c>
+      <c r="J162" s="3">
+        <v>1</v>
+      </c>
+      <c r="K162" s="3">
+        <v>0</v>
+      </c>
+      <c r="L162" s="3">
+        <v>1</v>
+      </c>
+      <c r="M162" s="3">
+        <v>0</v>
+      </c>
+      <c r="N162" s="3">
+        <v>0</v>
+      </c>
+      <c r="O162" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15">
+      <c r="A163" t="s">
+        <v>21</v>
+      </c>
+      <c r="B163" t="s">
+        <v>188</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>5</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+      <c r="H163" s="2">
+        <v>0</v>
+      </c>
+      <c r="I163" s="3">
+        <v>0</v>
+      </c>
+      <c r="J163" s="3">
+        <v>0</v>
+      </c>
+      <c r="K163" s="3">
+        <v>0</v>
+      </c>
+      <c r="L163" s="3">
+        <v>1</v>
+      </c>
+      <c r="M163" s="3">
+        <v>0</v>
+      </c>
+      <c r="N163" s="3">
+        <v>0</v>
+      </c>
+      <c r="O163" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15">
+      <c r="A164" t="s">
+        <v>20</v>
+      </c>
+      <c r="B164" t="s">
+        <v>189</v>
+      </c>
+      <c r="C164">
+        <v>0</v>
+      </c>
+      <c r="D164">
+        <v>3</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>5</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164" s="2">
+        <v>2</v>
+      </c>
+      <c r="I164" s="3">
+        <v>0</v>
+      </c>
+      <c r="J164" s="3">
+        <v>3</v>
+      </c>
+      <c r="K164" s="3">
+        <v>0</v>
+      </c>
+      <c r="L164" s="3">
+        <v>1</v>
+      </c>
+      <c r="M164" s="3">
+        <v>0</v>
+      </c>
+      <c r="N164" s="3">
+        <v>2</v>
+      </c>
+      <c r="O164" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15">
+      <c r="A165" t="s">
+        <v>21</v>
+      </c>
+      <c r="B165" t="s">
+        <v>190</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165" s="2">
+        <v>0</v>
+      </c>
+      <c r="I165" s="3">
+        <v>0</v>
+      </c>
+      <c r="J165" s="3">
+        <v>0</v>
+      </c>
+      <c r="K165" s="3">
+        <v>0</v>
+      </c>
+      <c r="L165" s="3">
+        <v>0</v>
+      </c>
+      <c r="M165" s="3">
+        <v>0</v>
+      </c>
+      <c r="N165" s="3">
+        <v>0</v>
+      </c>
+      <c r="O165" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
+      <c r="A166" t="s">
+        <v>21</v>
+      </c>
+      <c r="B166" t="s">
+        <v>191</v>
+      </c>
+      <c r="C166">
+        <v>0</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166" s="2">
+        <v>1</v>
+      </c>
+      <c r="I166" s="3">
+        <v>0</v>
+      </c>
+      <c r="J166" s="3">
+        <v>0</v>
+      </c>
+      <c r="K166" s="3">
+        <v>0</v>
+      </c>
+      <c r="L166" s="3">
+        <v>0</v>
+      </c>
+      <c r="M166">
+        <v>0</v>
+      </c>
+      <c r="N166" s="3">
+        <v>0</v>
+      </c>
+      <c r="O166" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15">
+      <c r="A167" t="s">
+        <v>26</v>
+      </c>
+      <c r="B167" t="s">
+        <v>192</v>
+      </c>
+      <c r="C167">
+        <v>0</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <v>1</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167" s="2">
+        <v>0</v>
+      </c>
+      <c r="I167" s="3">
+        <v>0</v>
+      </c>
+      <c r="J167" s="3">
+        <v>0</v>
+      </c>
+      <c r="K167" s="3">
+        <v>0</v>
+      </c>
+      <c r="L167" s="3">
+        <v>0</v>
+      </c>
+      <c r="M167">
+        <v>0</v>
+      </c>
+      <c r="N167" s="3">
+        <v>0</v>
+      </c>
+      <c r="O167" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15">
+      <c r="A168" t="s">
+        <v>26</v>
+      </c>
+      <c r="B168" t="s">
+        <v>193</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168" s="2">
+        <v>0</v>
+      </c>
+      <c r="I168" s="3">
+        <v>0</v>
+      </c>
+      <c r="J168" s="3">
+        <v>0</v>
+      </c>
+      <c r="K168" s="3">
+        <v>0</v>
+      </c>
+      <c r="L168" s="3">
+        <v>0</v>
+      </c>
+      <c r="M168">
+        <v>0</v>
+      </c>
+      <c r="N168" s="3">
+        <v>0</v>
+      </c>
+      <c r="O168" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15">
+      <c r="A169" t="s">
+        <v>20</v>
+      </c>
+      <c r="B169" t="s">
+        <v>194</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>2</v>
+      </c>
+      <c r="F169">
+        <v>3</v>
+      </c>
+      <c r="G169">
+        <v>2</v>
+      </c>
+      <c r="H169" s="2">
+        <v>2</v>
+      </c>
+      <c r="I169" s="3">
+        <v>1</v>
+      </c>
+      <c r="J169" s="3">
+        <v>1</v>
+      </c>
+      <c r="K169" s="3">
+        <v>2</v>
+      </c>
+      <c r="L169" s="3">
+        <v>0</v>
+      </c>
+      <c r="M169" s="3">
+        <v>0</v>
+      </c>
+      <c r="N169" s="3">
+        <v>1</v>
+      </c>
+      <c r="O169" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15">
+      <c r="A170" t="s">
+        <v>89</v>
+      </c>
+      <c r="B170" t="s">
+        <v>195</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>1</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170" s="2">
+        <v>1</v>
+      </c>
+      <c r="I170" s="3">
+        <v>0</v>
+      </c>
+      <c r="J170" s="3">
+        <v>0</v>
+      </c>
+      <c r="K170" s="3">
+        <v>0</v>
+      </c>
+      <c r="L170" s="3">
+        <v>0</v>
+      </c>
+      <c r="M170" s="3">
+        <v>0</v>
+      </c>
+      <c r="N170" s="3">
+        <v>1</v>
+      </c>
+      <c r="O170" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15">
+      <c r="A171" t="s">
+        <v>20</v>
+      </c>
+      <c r="B171" t="s">
+        <v>196</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>2</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171" s="2">
+        <v>0</v>
+      </c>
+      <c r="I171" s="3">
+        <v>0</v>
+      </c>
+      <c r="J171" s="3">
+        <v>0</v>
+      </c>
+      <c r="K171" s="3">
+        <v>1</v>
+      </c>
+      <c r="L171" s="3">
+        <v>0</v>
+      </c>
+      <c r="M171" s="3">
+        <v>0</v>
+      </c>
+      <c r="N171" s="3">
+        <v>0</v>
+      </c>
+      <c r="O171" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15">
+      <c r="A172" t="s">
+        <v>21</v>
+      </c>
+      <c r="B172" t="s">
+        <v>197</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>1</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172" s="2">
+        <v>0</v>
+      </c>
+      <c r="I172" s="3">
+        <v>0</v>
+      </c>
+      <c r="J172" s="3">
+        <v>0</v>
+      </c>
+      <c r="K172" s="3">
+        <v>0</v>
+      </c>
+      <c r="L172" s="3">
+        <v>0</v>
+      </c>
+      <c r="M172" s="3">
+        <v>0</v>
+      </c>
+      <c r="N172" s="3">
+        <v>0</v>
+      </c>
+      <c r="O172" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15">
+      <c r="A173" t="s">
+        <v>21</v>
+      </c>
+      <c r="B173" t="s">
+        <v>198</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>3</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173" s="2">
+        <v>2</v>
+      </c>
+      <c r="I173" s="3">
+        <v>0</v>
+      </c>
+      <c r="J173" s="3">
+        <v>0</v>
+      </c>
+      <c r="K173" s="3">
+        <v>0</v>
+      </c>
+      <c r="L173" s="3">
+        <v>1</v>
+      </c>
+      <c r="M173" s="3">
+        <v>0</v>
+      </c>
+      <c r="N173">
+        <v>1</v>
+      </c>
+      <c r="O173" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15">
+      <c r="A174" t="s">
+        <v>21</v>
+      </c>
+      <c r="B174" t="s">
+        <v>91</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>1</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174" s="2">
+        <v>0</v>
+      </c>
+      <c r="I174" s="3">
+        <v>0</v>
+      </c>
+      <c r="J174" s="3">
+        <v>0</v>
+      </c>
+      <c r="K174" s="3">
+        <v>0</v>
+      </c>
+      <c r="L174" s="3">
+        <v>0</v>
+      </c>
+      <c r="M174" s="3">
+        <v>0</v>
+      </c>
+      <c r="N174">
+        <v>0</v>
+      </c>
+      <c r="O174" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15">
+      <c r="A175" t="s">
+        <v>20</v>
+      </c>
+      <c r="B175" t="s">
+        <v>199</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
+      <c r="H175" s="2">
+        <v>1</v>
+      </c>
+      <c r="I175" s="3">
+        <v>0</v>
+      </c>
+      <c r="J175" s="3">
+        <v>0</v>
+      </c>
+      <c r="K175" s="3">
+        <v>0</v>
+      </c>
+      <c r="L175" s="3">
+        <v>0</v>
+      </c>
+      <c r="M175" s="3">
+        <v>0</v>
+      </c>
+      <c r="N175" s="3">
+        <v>0</v>
+      </c>
+      <c r="O175" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15">
+      <c r="A176" t="s">
+        <v>21</v>
+      </c>
+      <c r="B176" t="s">
+        <v>200</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>1</v>
+      </c>
+      <c r="H176" s="2">
+        <v>0</v>
+      </c>
+      <c r="I176" s="3">
+        <v>0</v>
+      </c>
+      <c r="J176" s="3">
+        <v>0</v>
+      </c>
+      <c r="K176" s="3">
+        <v>0</v>
+      </c>
+      <c r="L176" s="3">
+        <v>0</v>
+      </c>
+      <c r="M176" s="3">
+        <v>1</v>
+      </c>
+      <c r="N176" s="3">
+        <v>0</v>
+      </c>
+      <c r="O176" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15">
+      <c r="A177" t="s">
+        <v>26</v>
+      </c>
+      <c r="B177" t="s">
+        <v>136</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>1</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+      <c r="H177" s="2">
+        <v>0</v>
+      </c>
+      <c r="I177" s="3">
+        <v>0</v>
+      </c>
+      <c r="J177" s="3">
+        <v>0</v>
+      </c>
+      <c r="K177" s="3">
+        <v>0</v>
+      </c>
+      <c r="L177">
+        <v>1</v>
+      </c>
+      <c r="M177" s="3">
+        <v>0</v>
+      </c>
+      <c r="N177">
+        <v>0</v>
+      </c>
+      <c r="O177" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15">
+      <c r="A178" t="s">
+        <v>26</v>
+      </c>
+      <c r="B178" t="s">
+        <v>201</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>1</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178" s="1">
+        <v>0</v>
+      </c>
+      <c r="I178" s="3">
+        <v>0</v>
+      </c>
+      <c r="J178" s="3">
+        <v>0</v>
+      </c>
+      <c r="K178" s="3">
+        <v>0</v>
+      </c>
+      <c r="L178" s="3">
+        <v>0</v>
+      </c>
+      <c r="M178" s="3">
+        <v>0</v>
+      </c>
+      <c r="N178" s="3">
+        <v>0</v>
+      </c>
+      <c r="O178" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15">
+      <c r="A179" t="s">
+        <v>21</v>
+      </c>
+      <c r="B179" t="s">
+        <v>202</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>1</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
+      <c r="H179" s="1">
+        <v>2</v>
+      </c>
+      <c r="I179" s="3">
+        <v>0</v>
+      </c>
+      <c r="J179" s="3">
+        <v>0</v>
+      </c>
+      <c r="K179" s="3">
+        <v>0</v>
+      </c>
+      <c r="L179" s="3">
+        <v>0</v>
+      </c>
+      <c r="M179" s="3">
+        <v>0</v>
+      </c>
+      <c r="N179" s="3">
+        <v>1</v>
+      </c>
+      <c r="O179" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15">
+      <c r="A180" t="s">
+        <v>20</v>
+      </c>
+      <c r="B180" t="s">
+        <v>203</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>3</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>3</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180" s="1">
+        <v>0</v>
+      </c>
+      <c r="I180" s="3">
+        <v>0</v>
+      </c>
+      <c r="J180" s="3">
+        <v>1</v>
+      </c>
+      <c r="K180" s="3">
+        <v>1</v>
+      </c>
+      <c r="L180" s="3">
+        <v>3</v>
+      </c>
+      <c r="M180" s="3">
+        <v>0</v>
+      </c>
+      <c r="N180" s="3">
+        <v>0</v>
+      </c>
+      <c r="O180" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15">
+      <c r="A181" t="s">
+        <v>20</v>
+      </c>
+      <c r="B181" t="s">
+        <v>204</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>2</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>2</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181" s="1">
+        <v>3</v>
+      </c>
+      <c r="I181" s="3">
+        <v>0</v>
+      </c>
+      <c r="J181" s="3">
+        <v>0</v>
+      </c>
+      <c r="K181" s="3">
+        <v>0</v>
+      </c>
+      <c r="L181" s="3">
+        <v>1</v>
+      </c>
+      <c r="M181" s="3">
+        <v>0</v>
+      </c>
+      <c r="N181" s="3">
+        <v>2</v>
+      </c>
+      <c r="O181" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15">
+      <c r="A182" t="s">
+        <v>20</v>
+      </c>
+      <c r="B182" t="s">
+        <v>205</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>4</v>
+      </c>
+      <c r="E182">
+        <v>1</v>
+      </c>
+      <c r="F182">
+        <v>5</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182" s="1">
+        <v>2</v>
+      </c>
+      <c r="I182" s="3">
+        <v>0</v>
+      </c>
+      <c r="J182" s="3">
+        <v>1</v>
+      </c>
+      <c r="K182" s="3">
+        <v>0</v>
+      </c>
+      <c r="L182" s="3">
+        <v>1</v>
+      </c>
+      <c r="M182" s="3">
+        <v>0</v>
+      </c>
+      <c r="N182" s="3">
+        <v>1</v>
+      </c>
+      <c r="O182" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15">
+      <c r="A183" t="s">
+        <v>26</v>
+      </c>
+      <c r="B183" t="s">
+        <v>206</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>2</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183" s="1">
+        <v>1</v>
+      </c>
+      <c r="I183" s="3">
+        <v>0</v>
+      </c>
+      <c r="J183" s="3">
+        <v>0</v>
+      </c>
+      <c r="K183" s="3">
+        <v>0</v>
+      </c>
+      <c r="L183" s="3">
+        <v>0</v>
+      </c>
+      <c r="M183" s="3">
+        <v>0</v>
+      </c>
+      <c r="N183" s="3">
+        <v>0</v>
+      </c>
+      <c r="O183" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15">
+      <c r="A184" t="s">
+        <v>21</v>
+      </c>
+      <c r="B184" t="s">
+        <v>207</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>5</v>
+      </c>
+      <c r="E184">
+        <v>4</v>
+      </c>
+      <c r="F184">
+        <v>3</v>
+      </c>
+      <c r="G184">
+        <v>1</v>
+      </c>
+      <c r="H184" s="1">
+        <v>3</v>
+      </c>
+      <c r="I184" s="3">
+        <v>1</v>
+      </c>
+      <c r="J184" s="3">
+        <v>4</v>
+      </c>
+      <c r="K184" s="3">
+        <v>0</v>
+      </c>
+      <c r="L184" s="3">
+        <v>1</v>
+      </c>
+      <c r="M184" s="3">
+        <v>1</v>
+      </c>
+      <c r="N184" s="3">
+        <v>1</v>
+      </c>
+      <c r="O184" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15">
+      <c r="A185" t="s">
+        <v>26</v>
+      </c>
+      <c r="B185" t="s">
+        <v>208</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>1</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185" s="1">
+        <v>0</v>
+      </c>
+      <c r="I185" s="3">
+        <v>0</v>
+      </c>
+      <c r="J185" s="3">
+        <v>0</v>
+      </c>
+      <c r="K185" s="3">
+        <v>0</v>
+      </c>
+      <c r="L185" s="3">
+        <v>0</v>
+      </c>
+      <c r="M185" s="3">
+        <v>0</v>
+      </c>
+      <c r="N185" s="3">
+        <v>0</v>
+      </c>
+      <c r="O185" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15">
+      <c r="A186" t="s">
+        <v>21</v>
+      </c>
+      <c r="B186" t="s">
+        <v>209</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>2</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186" s="1">
+        <v>1</v>
+      </c>
+      <c r="I186" s="3">
+        <v>0</v>
+      </c>
+      <c r="J186" s="3">
+        <v>0</v>
+      </c>
+      <c r="K186" s="3">
+        <v>0</v>
+      </c>
+      <c r="L186" s="3">
+        <v>0</v>
+      </c>
+      <c r="M186" s="3">
+        <v>0</v>
+      </c>
+      <c r="N186" s="3">
+        <v>1</v>
+      </c>
+      <c r="O186" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15">
+      <c r="A187" t="s">
+        <v>21</v>
+      </c>
+      <c r="B187" t="s">
+        <v>210</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>1</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187" s="1">
+        <v>0</v>
+      </c>
+      <c r="I187" s="3">
+        <v>0</v>
+      </c>
+      <c r="J187" s="3">
+        <v>0</v>
+      </c>
+      <c r="K187" s="3">
+        <v>0</v>
+      </c>
+      <c r="L187" s="3">
+        <v>0</v>
+      </c>
+      <c r="M187" s="3">
+        <v>0</v>
+      </c>
+      <c r="N187" s="3">
+        <v>0</v>
+      </c>
+      <c r="O187" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15">
+      <c r="A188" t="s">
+        <v>26</v>
+      </c>
+      <c r="B188" t="s">
+        <v>216</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188">
+        <v>1</v>
+      </c>
+      <c r="G188">
+        <v>1</v>
+      </c>
+      <c r="H188" s="2">
+        <v>0</v>
+      </c>
+      <c r="I188" s="3">
+        <v>0</v>
+      </c>
+      <c r="J188" s="3">
+        <v>0</v>
+      </c>
+      <c r="K188" s="3">
+        <v>0</v>
+      </c>
+      <c r="L188" s="3">
+        <v>0</v>
+      </c>
+      <c r="M188" s="3">
+        <v>0</v>
+      </c>
+      <c r="N188" s="3">
+        <v>0</v>
+      </c>
+      <c r="O188" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15">
+      <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>217</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>2</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189">
+        <v>2</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189" s="2">
+        <v>3</v>
+      </c>
+      <c r="I189" s="3">
+        <v>0</v>
+      </c>
+      <c r="J189">
+        <v>2</v>
+      </c>
+      <c r="K189">
+        <v>1</v>
+      </c>
+      <c r="L189">
+        <v>1</v>
+      </c>
+      <c r="M189" s="3">
+        <v>0</v>
+      </c>
+      <c r="N189">
+        <v>2</v>
+      </c>
+      <c r="O189" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15">
+      <c r="A190" t="s">
+        <v>26</v>
+      </c>
+      <c r="B190" t="s">
+        <v>218</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>0</v>
+      </c>
+      <c r="F190">
+        <v>1</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190" s="2">
+        <v>0</v>
+      </c>
+      <c r="I190" s="3">
+        <v>0</v>
+      </c>
+      <c r="J190">
+        <v>1</v>
+      </c>
+      <c r="K190">
+        <v>0</v>
+      </c>
+      <c r="L190">
+        <v>0</v>
+      </c>
+      <c r="M190" s="3">
+        <v>0</v>
+      </c>
+      <c r="N190" s="3">
+        <v>0</v>
+      </c>
+      <c r="O190" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15">
+      <c r="A191" t="s">
+        <v>21</v>
+      </c>
+      <c r="B191" t="s">
+        <v>220</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191">
+        <v>1</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191" s="2">
+        <v>0</v>
+      </c>
+      <c r="I191" s="3">
+        <v>0</v>
+      </c>
+      <c r="J191" s="3">
+        <v>0</v>
+      </c>
+      <c r="K191">
+        <v>0</v>
+      </c>
+      <c r="L191">
+        <v>0</v>
+      </c>
+      <c r="M191" s="3">
+        <v>0</v>
+      </c>
+      <c r="N191" s="3">
+        <v>0</v>
+      </c>
+      <c r="O191" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15">
+      <c r="A192" t="s">
+        <v>21</v>
+      </c>
+      <c r="B192" t="s">
+        <v>221</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192">
+        <v>4</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192" s="2">
+        <v>3</v>
+      </c>
+      <c r="I192" s="3">
+        <v>0</v>
+      </c>
+      <c r="J192" s="3">
+        <v>0</v>
+      </c>
+      <c r="K192">
+        <v>0</v>
+      </c>
+      <c r="L192">
+        <v>0</v>
+      </c>
+      <c r="M192">
+        <v>0</v>
+      </c>
+      <c r="N192" s="3">
+        <v>0</v>
+      </c>
+      <c r="O192" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15">
+      <c r="A193" t="s">
+        <v>21</v>
+      </c>
+      <c r="B193" t="s">
+        <v>222</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>4</v>
+      </c>
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193">
+        <v>3</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193" s="2">
+        <v>3</v>
+      </c>
+      <c r="I193" s="3">
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>3</v>
+      </c>
+      <c r="K193">
+        <v>0</v>
+      </c>
+      <c r="L193">
+        <v>0</v>
+      </c>
+      <c r="M193">
+        <v>0</v>
+      </c>
+      <c r="N193">
+        <v>1</v>
+      </c>
+      <c r="O193" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15">
+      <c r="A194" t="s">
+        <v>21</v>
+      </c>
+      <c r="B194" t="s">
+        <v>223</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>3</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194">
+        <v>1</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194" s="2">
+        <v>0</v>
+      </c>
+      <c r="I194" s="3">
+        <v>0</v>
+      </c>
+      <c r="J194">
+        <v>1</v>
+      </c>
+      <c r="K194">
+        <v>0</v>
+      </c>
+      <c r="L194">
+        <v>0</v>
+      </c>
+      <c r="M194">
+        <v>0</v>
+      </c>
+      <c r="N194">
+        <v>0</v>
+      </c>
+      <c r="O194" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15">
+      <c r="A195" t="s">
+        <v>26</v>
+      </c>
+      <c r="B195" t="s">
+        <v>224</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195">
+        <v>0</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195" s="2">
+        <v>0</v>
+      </c>
+      <c r="I195" s="3">
+        <v>0</v>
+      </c>
+      <c r="J195" s="3">
+        <v>0</v>
+      </c>
+      <c r="K195">
+        <v>0</v>
+      </c>
+      <c r="L195">
+        <v>0</v>
+      </c>
+      <c r="M195">
+        <v>0</v>
+      </c>
+      <c r="N195">
+        <v>0</v>
+      </c>
+      <c r="O195" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15">
+      <c r="A196" t="s">
+        <v>20</v>
+      </c>
+      <c r="B196" t="s">
+        <v>227</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>0</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196" s="2">
+        <v>1</v>
+      </c>
+      <c r="I196" s="3">
+        <v>0</v>
+      </c>
+      <c r="J196" s="3">
+        <v>0</v>
+      </c>
+      <c r="K196">
+        <v>0</v>
+      </c>
+      <c r="L196">
+        <v>0</v>
+      </c>
+      <c r="M196">
+        <v>0</v>
+      </c>
+      <c r="N196">
+        <v>1</v>
+      </c>
+      <c r="O196" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15">
+      <c r="A197" t="s">
+        <v>21</v>
+      </c>
+      <c r="B197" t="s">
+        <v>225</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197" s="2">
+        <v>0</v>
+      </c>
+      <c r="I197" s="3">
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+      <c r="K197">
+        <v>0</v>
+      </c>
+      <c r="L197">
+        <v>0</v>
+      </c>
+      <c r="M197">
+        <v>0</v>
+      </c>
+      <c r="N197">
+        <v>0</v>
+      </c>
+      <c r="O197" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15">
+      <c r="A198" t="s">
+        <v>21</v>
+      </c>
+      <c r="B198" t="s">
+        <v>226</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198" s="2">
+        <v>1</v>
+      </c>
+      <c r="I198" s="3">
+        <v>0</v>
+      </c>
+      <c r="J198" s="3">
+        <v>0</v>
+      </c>
+      <c r="K198">
+        <v>0</v>
+      </c>
+      <c r="L198">
+        <v>0</v>
+      </c>
+      <c r="M198">
+        <v>0</v>
+      </c>
+      <c r="N198">
+        <v>0</v>
+      </c>
+      <c r="O198" t="s">
+        <v>219</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P128"/>
+  <autoFilter ref="A1:P177"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>